<commit_message>
Updated code with latest changes
</commit_message>
<xml_diff>
--- a/Odisha_biomass.xlsx
+++ b/Odisha_biomass.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBC3BBE-9335-4888-9269-F886B4E31F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683F33FB-02E4-4E09-AA4D-D3F9ECA51418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54CE7AF6-DF55-467E-91F4-12004A3F375B}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>Dhenkanal</t>
   </si>
   <si>
-    <t>Jagatsinghapur</t>
-  </si>
-  <si>
     <t>Sambalpur</t>
   </si>
   <si>
@@ -138,13 +135,16 @@
     <t>Surplus Biomass Kilo tonnes</t>
   </si>
   <si>
-    <t>Baleshwar</t>
-  </si>
-  <si>
-    <t>Baudh</t>
-  </si>
-  <si>
-    <t>Debagarh</t>
+    <t>Balasore</t>
+  </si>
+  <si>
+    <t>Jagatsinghpur</t>
+  </si>
+  <si>
+    <t>Deogarh</t>
+  </si>
+  <si>
+    <t>Boudh</t>
   </si>
 </sst>
 </file>
@@ -207,10 +207,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -550,7 +550,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -567,76 +567,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -741,7 +741,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2">
         <v>28.32</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2">
         <v>49.88</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2">
         <v>34.39</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2">
         <v>4.8</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2">
         <v>3.17</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2">
         <v>22.24</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>8.5299999999999994</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>21.92</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2">
         <v>2.13</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2">
         <v>45.99</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2">
         <v>9.9600000000000009</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="2">
         <v>60.3</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="2">
         <v>29.42</v>

</xml_diff>